<commit_message>
problema grafica y actualizacion runt mayo
</commit_message>
<xml_diff>
--- a/BD_actualizado.xlsx
+++ b/BD_actualizado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naran\Entornos_virtuales\Pronosticos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://globalymc-my.sharepoint.com/personal/xb00429_globalymc_com/Documents/Analítica de Datos/Scripts_Aplicaciones/Pronosticos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA09743-73E8-4512-A2FF-4D33E6420AA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{9EA09743-73E8-4512-A2FF-4D33E6420AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FE9018F-CEB1-4957-A029-E6713056B209}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5163179C-28B6-4BD3-8773-07D3C5F95EB7}"/>
   </bookViews>
@@ -149,15 +149,15 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={D4E40391-FB57-4E64-B35B-02E181470A36}</author>
+    <author>tc={CBF1B39E-36E1-4CF7-839F-34E1C65A3FC4}</author>
   </authors>
   <commentList>
-    <comment ref="D242" authorId="0" shapeId="0" xr:uid="{D4E40391-FB57-4E64-B35B-02E181470A36}">
+    <comment ref="D245" authorId="0" shapeId="0" xr:uid="{CBF1B39E-36E1-4CF7-839F-34E1C65A3FC4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
-    PIB GROWTH - Proyección Bancolombia</t>
+    PIB Growth analistas locales</t>
       </text>
     </comment>
   </commentList>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="61">
   <si>
     <t>FECHA</t>
   </si>
@@ -361,7 +361,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +383,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -411,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -519,6 +527,9 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2510,8 +2521,8 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D242" dT="2021-04-29T19:08:01.69" personId="{8363812F-1AC7-4F99-B918-47E1D6E913B5}" id="{D4E40391-FB57-4E64-B35B-02E181470A36}">
-    <text>PIB GROWTH - Proyección Bancolombia</text>
+  <threadedComment ref="D245" dT="2021-06-01T17:19:38.76" personId="{8363812F-1AC7-4F99-B918-47E1D6E913B5}" id="{CBF1B39E-36E1-4CF7-839F-34E1C65A3FC4}">
+    <text>PIB Growth analistas locales</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2521,10 +2532,10 @@
   <dimension ref="A1:W289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B225" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E244" sqref="E244"/>
+      <selection pane="bottomRight" activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16586,11 +16597,11 @@
         <v>5.5E-2</v>
       </c>
       <c r="D194" s="19">
-        <v>0.01</v>
+        <v>1.0189999999999999E-2</v>
       </c>
       <c r="E194" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.16200000000000001</v>
+        <v>0.16181000000000001</v>
       </c>
       <c r="F194" s="20">
         <v>2941</v>
@@ -16659,11 +16670,11 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="D195" s="19">
-        <v>0.01</v>
+        <v>1.0189999999999999E-2</v>
       </c>
       <c r="E195" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.14699999999999999</v>
+        <v>0.14681</v>
       </c>
       <c r="F195" s="20">
         <v>2880</v>
@@ -16732,11 +16743,11 @@
         <v>4.7E-2</v>
       </c>
       <c r="D196" s="19">
-        <v>0.01</v>
+        <v>1.0189999999999999E-2</v>
       </c>
       <c r="E196" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.13400000000000001</v>
+        <v>0.13381000000000001</v>
       </c>
       <c r="F196" s="20">
         <v>2942</v>
@@ -16805,11 +16816,11 @@
         <v>4.7E-2</v>
       </c>
       <c r="D197" s="17">
-        <v>1.0999999999999999E-2</v>
+        <v>1.2547000000000001E-2</v>
       </c>
       <c r="E197" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.125</v>
+        <v>0.12345300000000001</v>
       </c>
       <c r="F197" s="20">
         <v>2878</v>
@@ -16877,12 +16888,12 @@
       <c r="C198" s="19">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D198" s="19">
-        <v>1.0999999999999999E-2</v>
+      <c r="D198" s="17">
+        <v>1.2547000000000001E-2</v>
       </c>
       <c r="E198" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.127</v>
+        <v>0.12545300000000001</v>
       </c>
       <c r="F198" s="20">
         <v>2924</v>
@@ -16950,12 +16961,12 @@
       <c r="C199" s="19">
         <v>0.04</v>
       </c>
-      <c r="D199" s="19">
-        <v>1.0999999999999999E-2</v>
+      <c r="D199" s="17">
+        <v>1.2547000000000001E-2</v>
       </c>
       <c r="E199" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11600000000000001</v>
+        <v>0.114453</v>
       </c>
       <c r="F199" s="20">
         <v>2957</v>
@@ -17024,11 +17035,11 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="D200" s="17">
-        <v>1.2999999999999999E-2</v>
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="E200" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11800000000000001</v>
+        <v>0.11410000000000001</v>
       </c>
       <c r="F200" s="20">
         <v>3037</v>
@@ -17096,12 +17107,12 @@
       <c r="C201" s="19">
         <v>3.9E-2</v>
       </c>
-      <c r="D201" s="19">
-        <v>1.2999999999999999E-2</v>
+      <c r="D201" s="17">
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="E201" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11700000000000001</v>
+        <v>0.11310000000000001</v>
       </c>
       <c r="F201" s="20">
         <v>2973</v>
@@ -17169,12 +17180,12 @@
       <c r="C202" s="19">
         <v>0.04</v>
       </c>
-      <c r="D202" s="19">
-        <v>1.2999999999999999E-2</v>
+      <c r="D202" s="17">
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="E202" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11900000000000001</v>
+        <v>0.11510000000000001</v>
       </c>
       <c r="F202" s="20">
         <v>2917</v>
@@ -17243,11 +17254,11 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="D203" s="19">
-        <v>1.4E-2</v>
+        <v>1.4397E-2</v>
       </c>
       <c r="E203" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.113</v>
+        <v>0.11260300000000001</v>
       </c>
       <c r="F203" s="20">
         <v>2954</v>
@@ -17316,11 +17327,11 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="D204" s="19">
-        <v>1.4E-2</v>
+        <v>1.4397E-2</v>
       </c>
       <c r="E204" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.111</v>
+        <v>0.11060300000000001</v>
       </c>
       <c r="F204" s="20">
         <v>3013</v>
@@ -17389,11 +17400,11 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="D205" s="19">
-        <v>1.4E-2</v>
+        <v>1.4397E-2</v>
       </c>
       <c r="E205" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.113</v>
+        <v>0.11260300000000001</v>
       </c>
       <c r="F205" s="20">
         <v>2992</v>
@@ -17462,11 +17473,11 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D206" s="17">
-        <v>1.7999999999999999E-2</v>
+        <v>1.626E-2</v>
       </c>
       <c r="E206" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.13700000000000001</v>
+        <v>0.13874</v>
       </c>
       <c r="F206" s="20">
         <v>2869</v>
@@ -17534,12 +17545,12 @@
       <c r="C207" s="19">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D207" s="19">
-        <v>1.7999999999999999E-2</v>
+      <c r="D207" s="17">
+        <v>1.626E-2</v>
       </c>
       <c r="E207" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.12400000000000001</v>
+        <v>0.12574000000000002</v>
       </c>
       <c r="F207" s="20">
         <v>2860</v>
@@ -17607,12 +17618,12 @@
       <c r="C208" s="19">
         <v>3.1E-2</v>
       </c>
-      <c r="D208" s="19">
-        <v>1.7999999999999999E-2</v>
+      <c r="D208" s="17">
+        <v>1.626E-2</v>
       </c>
       <c r="E208" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.107</v>
+        <v>0.10874</v>
       </c>
       <c r="F208" s="20">
         <v>2848</v>
@@ -17681,11 +17692,11 @@
         <v>3.1E-2</v>
       </c>
       <c r="D209" s="17">
-        <v>2.8000000000000001E-2</v>
+        <v>2.7820000000000001E-2</v>
       </c>
       <c r="E209" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.8000000000000004E-2</v>
+        <v>9.8180000000000003E-2</v>
       </c>
       <c r="F209" s="20">
         <v>2766</v>
@@ -17753,12 +17764,12 @@
       <c r="C210" s="19">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D210" s="19">
-        <v>2.8000000000000001E-2</v>
+      <c r="D210" s="17">
+        <v>2.7820000000000001E-2</v>
       </c>
       <c r="E210" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10100000000000001</v>
+        <v>0.10118000000000001</v>
       </c>
       <c r="F210" s="20">
         <v>2862</v>
@@ -17826,12 +17837,12 @@
       <c r="C211" s="19">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D211" s="19">
-        <v>2.8000000000000001E-2</v>
+      <c r="D211" s="17">
+        <v>2.7820000000000001E-2</v>
       </c>
       <c r="E211" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.5000000000000001E-2</v>
+        <v>9.5180000000000001E-2</v>
       </c>
       <c r="F211" s="20">
         <v>2890</v>
@@ -17900,11 +17911,11 @@
         <v>3.1E-2</v>
       </c>
       <c r="D212" s="17">
-        <v>2.7E-2</v>
+        <v>2.8660000000000001E-2</v>
       </c>
       <c r="E212" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10100000000000001</v>
+        <v>9.9339999999999998E-2</v>
       </c>
       <c r="F212" s="20">
         <v>2885</v>
@@ -17972,12 +17983,12 @@
       <c r="C213" s="19">
         <v>3.1E-2</v>
       </c>
-      <c r="D213" s="19">
-        <v>2.7E-2</v>
+      <c r="D213" s="17">
+        <v>2.8660000000000001E-2</v>
       </c>
       <c r="E213" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.6000000000000002E-2</v>
+        <v>9.4339999999999993E-2</v>
       </c>
       <c r="F213" s="20">
         <v>2959</v>
@@ -18045,12 +18056,12 @@
       <c r="C214" s="19">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D214" s="19">
-        <v>2.7E-2</v>
+      <c r="D214" s="17">
+        <v>2.8660000000000001E-2</v>
       </c>
       <c r="E214" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.1</v>
+        <v>9.8339999999999997E-2</v>
       </c>
       <c r="F214" s="20">
         <v>3034</v>
@@ -18119,11 +18130,11 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="D215" s="17">
-        <v>2.7E-2</v>
+        <v>2.8979999999999999E-2</v>
       </c>
       <c r="E215" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.7000000000000003E-2</v>
+        <v>9.5019999999999993E-2</v>
       </c>
       <c r="F215" s="20">
         <v>3085</v>
@@ -18191,12 +18202,12 @@
       <c r="C216" s="19">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D216" s="19">
-        <v>2.7E-2</v>
+      <c r="D216" s="17">
+        <v>2.8979999999999999E-2</v>
       </c>
       <c r="E216" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.4E-2</v>
+        <v>9.2019999999999991E-2</v>
       </c>
       <c r="F216" s="20">
         <v>3194</v>
@@ -18264,12 +18275,12 @@
       <c r="C217" s="19">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D217" s="19">
-        <v>2.7E-2</v>
+      <c r="D217" s="17">
+        <v>2.8979999999999999E-2</v>
       </c>
       <c r="E217" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10200000000000001</v>
+        <v>0.10002</v>
       </c>
       <c r="F217" s="20">
         <v>3219</v>
@@ -18338,11 +18349,11 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="D218" s="17">
-        <v>2.9000000000000001E-2</v>
+        <v>3.5513000000000003E-2</v>
       </c>
       <c r="E218" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.13100000000000001</v>
+        <v>0.124487</v>
       </c>
       <c r="F218" s="20">
         <v>3165</v>
@@ -18410,12 +18421,12 @@
       <c r="C219" s="19">
         <v>0.03</v>
       </c>
-      <c r="D219" s="19">
-        <v>2.9000000000000001E-2</v>
+      <c r="D219" s="17">
+        <v>3.5513000000000003E-2</v>
       </c>
       <c r="E219" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11899999999999999</v>
+        <v>0.11248699999999999</v>
       </c>
       <c r="F219" s="13">
         <v>3116</v>
@@ -18483,12 +18494,12 @@
       <c r="C220" s="23">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="D220" s="19">
-        <v>2.9000000000000001E-2</v>
+      <c r="D220" s="17">
+        <v>3.5513000000000003E-2</v>
       </c>
       <c r="E220" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11100000000000002</v>
+        <v>0.10448700000000001</v>
       </c>
       <c r="F220" s="13">
         <v>3129</v>
@@ -18557,11 +18568,11 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="D221" s="17">
-        <v>3.1E-2</v>
+        <v>3.0668999999999998E-2</v>
       </c>
       <c r="E221" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10500000000000001</v>
+        <v>0.10533100000000001</v>
       </c>
       <c r="F221" s="13">
         <v>3156</v>
@@ -18629,12 +18640,12 @@
       <c r="C222" s="19">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D222" s="19">
-        <v>3.1E-2</v>
+      <c r="D222" s="17">
+        <v>3.0668999999999998E-2</v>
       </c>
       <c r="E222" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10700000000000001</v>
+        <v>0.10733100000000001</v>
       </c>
       <c r="F222" s="20">
         <v>3304</v>
@@ -18702,12 +18713,12 @@
       <c r="C223" s="19">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D223" s="19">
-        <v>3.1E-2</v>
+      <c r="D223" s="17">
+        <v>3.0668999999999998E-2</v>
       </c>
       <c r="E223" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.7000000000000003E-2</v>
+        <v>9.7331000000000001E-2</v>
       </c>
       <c r="F223" s="20">
         <v>3261</v>
@@ -18776,11 +18787,11 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D224" s="17">
-        <v>3.4000000000000002E-2</v>
+        <v>3.2487000000000002E-2</v>
       </c>
       <c r="E224" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11099999999999999</v>
+        <v>0.11251299999999999</v>
       </c>
       <c r="F224" s="20">
         <v>3207</v>
@@ -18848,12 +18859,12 @@
       <c r="C225" s="19">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D225" s="19">
-        <v>3.4000000000000002E-2</v>
+      <c r="D225" s="17">
+        <v>3.2487000000000002E-2</v>
       </c>
       <c r="E225" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.11199999999999999</v>
+        <v>0.11351299999999999</v>
       </c>
       <c r="F225" s="20">
         <v>3411</v>
@@ -18921,12 +18932,12 @@
       <c r="C226" s="19">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D226" s="19">
-        <v>3.4000000000000002E-2</v>
+      <c r="D226" s="17">
+        <v>3.2487000000000002E-2</v>
       </c>
       <c r="E226" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10599999999999998</v>
+        <v>0.10751299999999998</v>
       </c>
       <c r="F226" s="20">
         <v>3399</v>
@@ -18995,11 +19006,11 @@
         <v>3.9E-2</v>
       </c>
       <c r="D227" s="17">
-        <v>3.5000000000000003E-2</v>
+        <v>3.2730000000000002E-2</v>
       </c>
       <c r="E227" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10200000000000001</v>
+        <v>0.10427</v>
       </c>
       <c r="F227" s="20">
         <v>3433</v>
@@ -19067,12 +19078,12 @@
       <c r="C228" s="19">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D228" s="19">
-        <v>3.5000000000000003E-2</v>
+      <c r="D228" s="17">
+        <v>3.2730000000000002E-2</v>
       </c>
       <c r="E228" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.6000000000000002E-2</v>
+        <v>9.8269999999999996E-2</v>
       </c>
       <c r="F228" s="20">
         <v>3401</v>
@@ -19140,12 +19151,12 @@
       <c r="C229" s="19">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D229" s="19">
-        <v>3.5000000000000003E-2</v>
+      <c r="D229" s="17">
+        <v>3.2730000000000002E-2</v>
       </c>
       <c r="E229" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.8000000000000004E-2</v>
+        <v>0.10027</v>
       </c>
       <c r="F229" s="20">
         <v>3378</v>
@@ -19214,11 +19225,11 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="D230" s="19">
-        <v>1.4E-2</v>
+        <v>5.8580000000000004E-3</v>
       </c>
       <c r="E230" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.152</v>
+        <v>0.16014200000000001</v>
       </c>
       <c r="F230" s="20">
         <v>3311</v>
@@ -19287,11 +19298,11 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="D231" s="19">
-        <v>1.4E-2</v>
+        <v>5.8580000000000004E-3</v>
       </c>
       <c r="E231" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.14499999999999999</v>
+        <v>0.153142</v>
       </c>
       <c r="F231" s="13">
         <v>3411</v>
@@ -19360,11 +19371,11 @@
         <v>3.9E-2</v>
       </c>
       <c r="D232" s="19">
-        <v>1.4E-2</v>
+        <v>5.8580000000000004E-3</v>
       </c>
       <c r="E232" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.151</v>
+        <v>0.15914200000000001</v>
       </c>
       <c r="F232" s="13">
         <v>3877</v>
@@ -19433,11 +19444,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D233" s="26">
-        <v>-0.157</v>
+        <v>-0.1573</v>
       </c>
       <c r="E233" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.39</v>
+        <v>0.39029999999999998</v>
       </c>
       <c r="F233" s="13">
         <v>3977</v>
@@ -19506,11 +19517,11 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="D234" s="26">
-        <v>-0.157</v>
+        <v>-0.1573</v>
       </c>
       <c r="E234" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.4</v>
+        <v>0.40029999999999999</v>
       </c>
       <c r="F234" s="13">
         <v>3858</v>
@@ -19579,11 +19590,11 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="D235" s="26">
-        <v>-0.157</v>
+        <v>-0.1573</v>
       </c>
       <c r="E235" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.377</v>
+        <v>0.37729999999999997</v>
       </c>
       <c r="F235" s="13">
         <v>3702</v>
@@ -19652,11 +19663,11 @@
         <v>0.02</v>
       </c>
       <c r="D236" s="26">
-        <v>-8.5000000000000006E-2</v>
+        <v>-8.3599999999999994E-2</v>
       </c>
       <c r="E236" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.307</v>
+        <v>0.30559999999999998</v>
       </c>
       <c r="F236" s="13">
         <v>3658</v>
@@ -19725,11 +19736,11 @@
         <v>1.9E-2</v>
       </c>
       <c r="D237" s="26">
-        <v>-8.5000000000000006E-2</v>
+        <v>-8.3599999999999994E-2</v>
       </c>
       <c r="E237" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.27200000000000002</v>
+        <v>0.27060000000000001</v>
       </c>
       <c r="F237" s="13">
         <v>3783</v>
@@ -19798,11 +19809,11 @@
         <v>0.02</v>
       </c>
       <c r="D238" s="26">
-        <v>-8.5000000000000006E-2</v>
+        <v>-8.3599999999999994E-2</v>
       </c>
       <c r="E238" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.26300000000000001</v>
+        <v>0.2616</v>
       </c>
       <c r="F238" s="13">
         <v>3750</v>
@@ -19871,11 +19882,11 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D239" s="26">
-        <v>-6.9000000000000006E-2</v>
+        <v>-3.6200000000000003E-2</v>
       </c>
       <c r="E239" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.23399999999999999</v>
+        <v>0.20119999999999999</v>
       </c>
       <c r="F239" s="13">
         <v>3834</v>
@@ -19944,11 +19955,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D240" s="26">
-        <v>-6.9000000000000006E-2</v>
+        <v>-3.6200000000000003E-2</v>
       </c>
       <c r="E240" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.21700000000000003</v>
+        <v>0.18420000000000003</v>
       </c>
       <c r="F240" s="13">
         <v>3686</v>
@@ -20017,11 +20028,11 @@
         <v>1.6E-2</v>
       </c>
       <c r="D241" s="26">
-        <v>-6.9000000000000006E-2</v>
+        <v>-3.6200000000000003E-2</v>
       </c>
       <c r="E241" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.21900000000000003</v>
+        <v>0.18620000000000003</v>
       </c>
       <c r="F241" s="13">
         <v>3466</v>
@@ -20090,11 +20101,11 @@
         <v>1.6E-2</v>
       </c>
       <c r="D242" s="26">
-        <v>5.5E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E242" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.13400000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="F242" s="13">
         <v>3491</v>
@@ -20163,11 +20174,11 @@
         <v>1.6E-2</v>
       </c>
       <c r="D243" s="26">
-        <v>5.5E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E243" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.12</v>
+        <v>0.16399999999999998</v>
       </c>
       <c r="F243" s="13">
         <v>3555</v>
@@ -20236,11 +20247,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D244" s="26">
-        <v>5.5E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E244" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>0.10199999999999998</v>
+        <v>0.14599999999999996</v>
       </c>
       <c r="F244" s="13">
         <v>3613</v>
@@ -20302,16 +20313,37 @@
       <c r="A245" s="8">
         <v>44287</v>
       </c>
-      <c r="B245" s="23"/>
-      <c r="C245" s="23"/>
-      <c r="D245" s="26"/>
-      <c r="E245" s="19"/>
-      <c r="F245" s="13"/>
-      <c r="G245" s="24"/>
-      <c r="H245" s="22"/>
-      <c r="I245" s="22"/>
-      <c r="J245" s="22"/>
-      <c r="K245" s="22"/>
+      <c r="B245" s="23">
+        <v>0.151</v>
+      </c>
+      <c r="C245" s="23">
+        <v>1.95E-2</v>
+      </c>
+      <c r="D245" s="26">
+        <v>4.0999999999999995E-2</v>
+      </c>
+      <c r="E245" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>0.1295</v>
+      </c>
+      <c r="F245" s="13">
+        <v>3735.67</v>
+      </c>
+      <c r="G245" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H245" s="22">
+        <v>-0.34200000000000003</v>
+      </c>
+      <c r="I245" s="22">
+        <v>-0.23300000000000001</v>
+      </c>
+      <c r="J245" s="22">
+        <v>-0.505</v>
+      </c>
+      <c r="K245" s="22">
+        <v>61.7</v>
+      </c>
       <c r="L245" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>4</v>
@@ -20351,7 +20383,7 @@
       </c>
     </row>
     <row r="246" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A246" s="8">
+      <c r="A246" s="40">
         <v>44317</v>
       </c>
       <c r="B246" s="23"/>
@@ -20374,14 +20406,33 @@
       <c r="N246" s="14">
         <v>2</v>
       </c>
-      <c r="O246" s="15"/>
-      <c r="P246" s="15"/>
-      <c r="Q246" s="16"/>
-      <c r="R246" s="16"/>
-      <c r="S246" s="16"/>
-      <c r="T246" s="16"/>
-      <c r="U246" s="24"/>
-      <c r="W246" s="24"/>
+      <c r="O246" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="P246" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q246" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R246" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S246" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T246" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="U246" s="24">
+        <v>45169</v>
+      </c>
+      <c r="V246" s="14">
+        <v>8517</v>
+      </c>
+      <c r="W246" s="24">
+        <v>8616</v>
+      </c>
     </row>
     <row r="247" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A247" s="8">

</xml_diff>

<commit_message>
actualizacion datos junio y julio
</commit_message>
<xml_diff>
--- a/BD_actualizado.xlsx
+++ b/BD_actualizado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://globalymc-my.sharepoint.com/personal/xb00429_globalymc_com/Documents/Analítica de Datos/Scripts_Aplicaciones/Pronosticos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naran\Entornos_virtuales\Pronosticos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{9EA09743-73E8-4512-A2FF-4D33E6420AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FE9018F-CEB1-4957-A029-E6713056B209}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3609658-AA60-4430-9154-0F300A5C566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5163179C-28B6-4BD3-8773-07D3C5F95EB7}"/>
   </bookViews>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="61">
   <si>
     <t>FECHA</t>
   </si>
@@ -361,7 +361,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,14 +383,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -528,7 +520,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2532,10 +2524,10 @@
   <dimension ref="A1:W289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B225" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B228" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A246" sqref="A246"/>
+      <selection pane="bottomRight" activeCell="A248" sqref="A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20327,7 +20319,7 @@
         <v>0.1295</v>
       </c>
       <c r="F245" s="13">
-        <v>3735.67</v>
+        <v>3650.78</v>
       </c>
       <c r="G245" s="24">
         <v>1014980</v>
@@ -20342,7 +20334,7 @@
         <v>-0.505</v>
       </c>
       <c r="K245" s="22">
-        <v>61.7</v>
+        <v>63.58</v>
       </c>
       <c r="L245" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
@@ -20386,16 +20378,37 @@
       <c r="A246" s="40">
         <v>44317</v>
       </c>
-      <c r="B246" s="23"/>
-      <c r="C246" s="23"/>
-      <c r="D246" s="26"/>
-      <c r="E246" s="19"/>
-      <c r="F246" s="13"/>
-      <c r="G246" s="24"/>
-      <c r="H246" s="22"/>
-      <c r="I246" s="22"/>
-      <c r="J246" s="22"/>
-      <c r="K246" s="22"/>
+      <c r="B246" s="23">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="C246" s="23">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D246" s="26">
+        <v>4.0999999999999995E-2</v>
+      </c>
+      <c r="E246" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>0.14829999999999999</v>
+      </c>
+      <c r="F246" s="13">
+        <v>3735.67</v>
+      </c>
+      <c r="G246" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H246" s="22">
+        <v>-0.34300000000000003</v>
+      </c>
+      <c r="I246" s="22">
+        <v>-0.16</v>
+      </c>
+      <c r="J246" s="22">
+        <v>-0.61699999999999999</v>
+      </c>
+      <c r="K246" s="22">
+        <v>66.319999999999993</v>
+      </c>
       <c r="L246" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>5</v>
@@ -20438,16 +20451,37 @@
       <c r="A247" s="8">
         <v>44348</v>
       </c>
-      <c r="B247" s="23"/>
-      <c r="C247" s="23"/>
-      <c r="D247" s="26"/>
-      <c r="E247" s="19"/>
-      <c r="F247" s="13"/>
-      <c r="G247" s="24"/>
-      <c r="H247" s="22"/>
-      <c r="I247" s="22"/>
-      <c r="J247" s="22"/>
-      <c r="K247" s="22"/>
+      <c r="B247" s="23">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C247" s="23">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="D247" s="26">
+        <v>4.0999999999999995E-2</v>
+      </c>
+      <c r="E247" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>0.13929999999999998</v>
+      </c>
+      <c r="F247" s="13">
+        <v>3685.04</v>
+      </c>
+      <c r="G247" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H247" s="22">
+        <v>-0.223</v>
+      </c>
+      <c r="I247" s="22">
+        <v>-4.5999999999999999E-2</v>
+      </c>
+      <c r="J247" s="22">
+        <v>-0.48799999999999999</v>
+      </c>
+      <c r="K247" s="22">
+        <v>73.47</v>
+      </c>
       <c r="L247" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>6</v>
@@ -20458,29 +20492,64 @@
       <c r="N247" s="14">
         <v>2</v>
       </c>
-      <c r="O247" s="15"/>
-      <c r="P247" s="15"/>
-      <c r="Q247" s="16"/>
-      <c r="R247" s="16"/>
-      <c r="S247" s="16"/>
-      <c r="T247" s="16"/>
-      <c r="U247" s="24"/>
-      <c r="W247" s="24"/>
+      <c r="O247" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="P247" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q247" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R247" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="S247" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T247" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="U247" s="24">
+        <v>60248</v>
+      </c>
+      <c r="V247" s="14">
+        <v>11235</v>
+      </c>
+      <c r="W247" s="24">
+        <v>10803</v>
+      </c>
     </row>
     <row r="248" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A248" s="8">
         <v>44378</v>
       </c>
       <c r="B248" s="23"/>
-      <c r="C248" s="23"/>
-      <c r="D248" s="26"/>
+      <c r="C248" s="23">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="D248" s="26">
+        <v>4.0999999999999995E-2</v>
+      </c>
       <c r="E248" s="19"/>
-      <c r="F248" s="13"/>
-      <c r="G248" s="24"/>
-      <c r="H248" s="22"/>
-      <c r="I248" s="22"/>
-      <c r="J248" s="22"/>
-      <c r="K248" s="22"/>
+      <c r="F248" s="13">
+        <v>3829.42</v>
+      </c>
+      <c r="G248" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H248" s="22">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="I248" s="22">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="J248" s="22">
+        <v>-0.317</v>
+      </c>
+      <c r="K248" s="22">
+        <v>73.95</v>
+      </c>
       <c r="L248" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>7</v>
@@ -20491,14 +20560,33 @@
       <c r="N248" s="14">
         <v>2</v>
       </c>
-      <c r="O248" s="15"/>
-      <c r="P248" s="15"/>
-      <c r="Q248" s="16"/>
-      <c r="R248" s="16"/>
-      <c r="S248" s="16"/>
-      <c r="T248" s="16"/>
-      <c r="U248" s="24"/>
-      <c r="W248" s="24"/>
+      <c r="O248" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="P248" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q248" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="R248" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="S248" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T248" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="U248" s="24">
+        <v>70444</v>
+      </c>
+      <c r="V248" s="14">
+        <v>12763</v>
+      </c>
+      <c r="W248" s="24">
+        <v>12433</v>
+      </c>
     </row>
     <row r="249" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A249" s="8">

</xml_diff>

<commit_message>
actualizacion base de datos en excel
</commit_message>
<xml_diff>
--- a/BD_actualizado.xlsx
+++ b/BD_actualizado.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://globalymc-my.sharepoint.com/personal/xb00429_globalymc_com/Documents/Analítica de Datos/Scripts_Aplicaciones/Pronosticos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cortiz.INCOLMOTOSYMCO\OneDrive - YAMAHA MOTOR CO., LTD\Analítica de Datos\Scripts_Aplicaciones\Pronosticos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{D3609658-AA60-4430-9154-0F300A5C566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A39EC8F-B6A9-4219-91A0-B143EF8559B7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5163179C-28B6-4BD3-8773-07D3C5F95EB7}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores mensuales" sheetId="1" r:id="rId1"/>
@@ -128,7 +127,7 @@
     <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">TRUE</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="61">
   <si>
     <t>FECHA</t>
   </si>
@@ -335,39 +334,53 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
+    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -393,9 +406,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -404,10 +417,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -417,16 +430,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -435,74 +448,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -527,7 +543,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -552,7 +568,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -577,7 +593,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -694,7 +710,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -719,7 +735,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -783,7 +799,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -793,7 +809,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -803,7 +819,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -813,7 +829,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -838,7 +854,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="0_);[Red]\(0\)"/>
+      <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -873,7 +889,7 @@
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -883,7 +899,7 @@
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -908,7 +924,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -933,7 +949,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="0.000"/>
+      <numFmt numFmtId="179" formatCode="0.000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -943,7 +959,7 @@
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2158,35 +2174,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D3C23F2-D122-4477-B9FC-BE416F57F1F2}" name="Tabla33" displayName="Tabla33" ref="A1:W289" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla33" displayName="Tabla33" ref="A1:W289" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{2B3177C5-6C86-4951-A7A2-D8E7BF06BF32}" name="FECHA" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{2CC3A4F0-D046-4B41-9824-4664F6198644}" name="DESEMPLEO" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{0F5704DB-EDFA-42B9-BEAF-6F43D9E93B7B}" name="INFLATION" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{C95F8DF2-7519-4304-8CDC-C52FBA59801F}" name="PIB GROWTH" dataDxfId="19" dataCellStyle="Porcentaje"/>
-    <tableColumn id="11" xr3:uid="{58E7B9B3-6AEE-4ECC-A09B-484B1B911E15}" name="ISM" dataDxfId="18" dataCellStyle="Porcentaje">
+    <tableColumn id="1" name="FECHA" dataDxfId="22"/>
+    <tableColumn id="2" name="DESEMPLEO" dataDxfId="21"/>
+    <tableColumn id="3" name="INFLATION" dataDxfId="20"/>
+    <tableColumn id="8" name="PIB GROWTH" dataDxfId="19" dataCellStyle="Porcentaje"/>
+    <tableColumn id="11" name="ISM" dataDxfId="18" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E43FE906-20C1-4F9A-B8D3-06B726B35036}" name="TRM" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{6DEDEC46-6B41-4157-BD87-1A99BEFF9A54}" name="SMMLV&amp;TTE" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{67A7B7C3-6CDD-4EB0-80C1-60868F135089}" name="ICC" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{BC2A44B0-986A-4F57-B6D5-186FC647094F}" name="IEE" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{0DF9B827-80E7-44D7-A34A-C3B5103523A6}" name="ICE" dataDxfId="13"/>
-    <tableColumn id="21" xr3:uid="{126CDEE4-5718-4659-AD1F-3F0F958D0AB3}" name="OIL PRICE" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{54214B95-9BBA-4175-A8FA-2CA9C1DE836E}" name="MES" dataDxfId="11">
+    <tableColumn id="9" name="TRM" dataDxfId="17"/>
+    <tableColumn id="7" name="SMMLV&amp;TTE" dataDxfId="16"/>
+    <tableColumn id="5" name="ICC" dataDxfId="15"/>
+    <tableColumn id="12" name="IEE" dataDxfId="14"/>
+    <tableColumn id="13" name="ICE" dataDxfId="13"/>
+    <tableColumn id="21" name="OIL PRICE" dataDxfId="12"/>
+    <tableColumn id="4" name="MES" dataDxfId="11">
       <calculatedColumnFormula>+MONTH(Tabla33[[#This Row],[FECHA]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2DF2DC83-D053-4FC7-B745-C399F0F07C87}" name="DIAS HABILES" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{03A03AC3-FD90-47F1-A476-B6DC86F3335B}" name="FESTIVOS" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{DAE73628-9924-4EBB-B3CB-70A2A5FABAB1}" name="TEMPORADA" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{44A04ACF-974D-4C2E-A241-A10950587507}" name="VACACIONES" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{2F794DB1-D100-47F9-9B66-8921ED7FC2EF}" name="CLIMA" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{2CAE14F3-CB55-40D3-8B87-16381750EBF0}" name="INGRESOS" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{D7B15810-7C80-4F43-AE5A-BA88402D2AAA}" name="PRECIOS" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{D333F6C9-61C7-4F20-A62E-3D1633CD2EA7}" name="IMPUESTOS" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{EEDD6905-B7A2-432F-ACB2-62F3910F376C}" name="RUNT MERCADO" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{9DA9DA5B-8FD1-4216-A52F-9FF70F38E242}" name="RUNT YAMAHA" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{09777F57-D302-4346-9E2F-E21603AA434A}" name="WHOLESALE" dataDxfId="0"/>
+    <tableColumn id="22" name="DIAS HABILES" dataDxfId="10"/>
+    <tableColumn id="25" name="FESTIVOS" dataDxfId="9"/>
+    <tableColumn id="6" name="TEMPORADA" dataDxfId="8"/>
+    <tableColumn id="10" name="VACACIONES" dataDxfId="7"/>
+    <tableColumn id="16" name="CLIMA" dataDxfId="6"/>
+    <tableColumn id="17" name="INGRESOS" dataDxfId="5"/>
+    <tableColumn id="18" name="PRECIOS" dataDxfId="4"/>
+    <tableColumn id="19" name="IMPUESTOS" dataDxfId="3"/>
+    <tableColumn id="14" name="RUNT MERCADO" dataDxfId="2"/>
+    <tableColumn id="15" name="RUNT YAMAHA" dataDxfId="1"/>
+    <tableColumn id="20" name="WHOLESALE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2488,38 +2504,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BFEB52-1FC1-498E-A4BF-49960519718C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B225" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B234" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K251" sqref="K251"/>
+      <selection pane="bottomRight" activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="36" customWidth="1"/>
+    <col min="1" max="1" width="19.375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="36" customWidth="1"/>
     <col min="3" max="3" width="15" style="37" customWidth="1"/>
     <col min="4" max="4" width="15" style="14" customWidth="1"/>
     <col min="5" max="5" width="15" style="38" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="10" max="11" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.875" customWidth="1"/>
+    <col min="10" max="11" width="13.125" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="29.6640625" style="25" customWidth="1"/>
-    <col min="16" max="16" width="24.88671875" style="25" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" style="25" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" style="39" customWidth="1"/>
-    <col min="19" max="19" width="17.5546875" style="38" customWidth="1"/>
-    <col min="20" max="20" width="35.44140625" style="14" customWidth="1"/>
-    <col min="21" max="23" width="16.33203125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="14" max="14" width="13.375" customWidth="1"/>
+    <col min="15" max="15" width="29.625" style="25" customWidth="1"/>
+    <col min="16" max="16" width="24.875" style="25" customWidth="1"/>
+    <col min="17" max="17" width="13.5" style="25" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="39" customWidth="1"/>
+    <col min="19" max="19" width="17.5" style="38" customWidth="1"/>
+    <col min="20" max="20" width="35.5" style="14" customWidth="1"/>
+    <col min="21" max="23" width="16.375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="7" customFormat="1">
       <c r="A2" s="8">
         <v>36892</v>
       </c>
@@ -2657,7 +2673,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" s="7" customFormat="1">
       <c r="A3" s="8">
         <v>36923</v>
       </c>
@@ -2724,7 +2740,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" s="7" customFormat="1">
       <c r="A4" s="8">
         <v>36951</v>
       </c>
@@ -2791,7 +2807,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" s="7" customFormat="1">
       <c r="A5" s="8">
         <v>36982</v>
       </c>
@@ -2858,7 +2874,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" s="7" customFormat="1">
       <c r="A6" s="8">
         <v>37012</v>
       </c>
@@ -2925,7 +2941,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" s="7" customFormat="1">
       <c r="A7" s="8">
         <v>37043</v>
       </c>
@@ -2992,7 +3008,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" s="7" customFormat="1">
       <c r="A8" s="8">
         <v>37073</v>
       </c>
@@ -3059,7 +3075,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" s="7" customFormat="1">
       <c r="A9" s="8">
         <v>37104</v>
       </c>
@@ -3126,7 +3142,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" s="7" customFormat="1">
       <c r="A10" s="8">
         <v>37135</v>
       </c>
@@ -3193,7 +3209,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" s="7" customFormat="1">
       <c r="A11" s="8">
         <v>37165</v>
       </c>
@@ -3260,7 +3276,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" s="7" customFormat="1">
       <c r="A12" s="8">
         <v>37196</v>
       </c>
@@ -3333,7 +3349,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" s="7" customFormat="1">
       <c r="A13" s="8">
         <v>37226</v>
       </c>
@@ -3406,7 +3422,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" s="7" customFormat="1">
       <c r="A14" s="8">
         <v>37257</v>
       </c>
@@ -3479,7 +3495,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" s="7" customFormat="1">
       <c r="A15" s="8">
         <v>37288</v>
       </c>
@@ -3552,7 +3568,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" s="7" customFormat="1">
       <c r="A16" s="8">
         <v>37316</v>
       </c>
@@ -3625,7 +3641,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" s="7" customFormat="1">
       <c r="A17" s="8">
         <v>37347</v>
       </c>
@@ -3698,7 +3714,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" s="7" customFormat="1">
       <c r="A18" s="8">
         <v>37377</v>
       </c>
@@ -3771,7 +3787,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" s="7" customFormat="1">
       <c r="A19" s="8">
         <v>37408</v>
       </c>
@@ -3844,7 +3860,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" s="7" customFormat="1">
       <c r="A20" s="8">
         <v>37438</v>
       </c>
@@ -3917,7 +3933,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" s="7" customFormat="1">
       <c r="A21" s="8">
         <v>37469</v>
       </c>
@@ -3990,7 +4006,7 @@
         <v>2442</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" s="7" customFormat="1">
       <c r="A22" s="8">
         <v>37500</v>
       </c>
@@ -4063,7 +4079,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" s="7" customFormat="1">
       <c r="A23" s="8">
         <v>37530</v>
       </c>
@@ -4136,7 +4152,7 @@
         <v>2547</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" s="7" customFormat="1">
       <c r="A24" s="8">
         <v>37561</v>
       </c>
@@ -4209,7 +4225,7 @@
         <v>2211</v>
       </c>
     </row>
-    <row r="25" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" s="7" customFormat="1">
       <c r="A25" s="8">
         <v>37591</v>
       </c>
@@ -4282,7 +4298,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" s="7" customFormat="1">
       <c r="A26" s="8">
         <v>37622</v>
       </c>
@@ -4355,7 +4371,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" s="7" customFormat="1">
       <c r="A27" s="8">
         <v>37653</v>
       </c>
@@ -4428,7 +4444,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" s="7" customFormat="1">
       <c r="A28" s="8">
         <v>37681</v>
       </c>
@@ -4501,7 +4517,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" s="7" customFormat="1">
       <c r="A29" s="8">
         <v>37712</v>
       </c>
@@ -4574,7 +4590,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" s="7" customFormat="1">
       <c r="A30" s="8">
         <v>37742</v>
       </c>
@@ -4647,7 +4663,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" s="7" customFormat="1">
       <c r="A31" s="8">
         <v>37773</v>
       </c>
@@ -4720,7 +4736,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" s="7" customFormat="1">
       <c r="A32" s="8">
         <v>37803</v>
       </c>
@@ -4793,7 +4809,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" s="7" customFormat="1">
       <c r="A33" s="8">
         <v>37834</v>
       </c>
@@ -4866,7 +4882,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" s="7" customFormat="1">
       <c r="A34" s="8">
         <v>37865</v>
       </c>
@@ -4939,7 +4955,7 @@
         <v>2940</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" s="7" customFormat="1">
       <c r="A35" s="8">
         <v>37895</v>
       </c>
@@ -5012,7 +5028,7 @@
         <v>2972</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" s="7" customFormat="1">
       <c r="A36" s="8">
         <v>37926</v>
       </c>
@@ -5085,7 +5101,7 @@
         <v>2717</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" s="7" customFormat="1">
       <c r="A37" s="8">
         <v>37956</v>
       </c>
@@ -5158,7 +5174,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" s="7" customFormat="1">
       <c r="A38" s="8">
         <v>37987</v>
       </c>
@@ -5231,7 +5247,7 @@
         <v>2591</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" s="7" customFormat="1">
       <c r="A39" s="8">
         <v>38018</v>
       </c>
@@ -5304,7 +5320,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" s="7" customFormat="1">
       <c r="A40" s="8">
         <v>38047</v>
       </c>
@@ -5377,7 +5393,7 @@
         <v>2618</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" s="7" customFormat="1">
       <c r="A41" s="8">
         <v>38078</v>
       </c>
@@ -5450,7 +5466,7 @@
         <v>2773</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" s="7" customFormat="1">
       <c r="A42" s="8">
         <v>38108</v>
       </c>
@@ -5523,7 +5539,7 @@
         <v>3091</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" s="7" customFormat="1">
       <c r="A43" s="8">
         <v>38139</v>
       </c>
@@ -5596,7 +5612,7 @@
         <v>3206</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" s="7" customFormat="1">
       <c r="A44" s="8">
         <v>38169</v>
       </c>
@@ -5669,7 +5685,7 @@
         <v>3401</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" s="7" customFormat="1">
       <c r="A45" s="8">
         <v>38200</v>
       </c>
@@ -5742,7 +5758,7 @@
         <v>4012</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" s="7" customFormat="1">
       <c r="A46" s="8">
         <v>38231</v>
       </c>
@@ -5815,7 +5831,7 @@
         <v>4410</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" s="7" customFormat="1">
       <c r="A47" s="8">
         <v>38261</v>
       </c>
@@ -5888,7 +5904,7 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="48" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" s="7" customFormat="1">
       <c r="A48" s="8">
         <v>38292</v>
       </c>
@@ -5961,7 +5977,7 @@
         <v>3864</v>
       </c>
     </row>
-    <row r="49" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" s="7" customFormat="1">
       <c r="A49" s="8">
         <v>38322</v>
       </c>
@@ -6034,7 +6050,7 @@
         <v>4331</v>
       </c>
     </row>
-    <row r="50" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" s="7" customFormat="1">
       <c r="A50" s="8">
         <v>38353</v>
       </c>
@@ -6107,7 +6123,7 @@
         <v>3682</v>
       </c>
     </row>
-    <row r="51" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" s="7" customFormat="1">
       <c r="A51" s="8">
         <v>38384</v>
       </c>
@@ -6180,7 +6196,7 @@
         <v>4104</v>
       </c>
     </row>
-    <row r="52" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" s="7" customFormat="1">
       <c r="A52" s="8">
         <v>38412</v>
       </c>
@@ -6253,7 +6269,7 @@
         <v>4275</v>
       </c>
     </row>
-    <row r="53" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" s="7" customFormat="1">
       <c r="A53" s="8">
         <v>38443</v>
       </c>
@@ -6326,7 +6342,7 @@
         <v>4334</v>
       </c>
     </row>
-    <row r="54" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" s="7" customFormat="1">
       <c r="A54" s="8">
         <v>38473</v>
       </c>
@@ -6399,7 +6415,7 @@
         <v>4033</v>
       </c>
     </row>
-    <row r="55" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" s="7" customFormat="1">
       <c r="A55" s="8">
         <v>38504</v>
       </c>
@@ -6472,7 +6488,7 @@
         <v>4708</v>
       </c>
     </row>
-    <row r="56" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" s="7" customFormat="1">
       <c r="A56" s="8">
         <v>38534</v>
       </c>
@@ -6545,7 +6561,7 @@
         <v>4450</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" s="7" customFormat="1">
       <c r="A57" s="8">
         <v>38565</v>
       </c>
@@ -6618,7 +6634,7 @@
         <v>5290</v>
       </c>
     </row>
-    <row r="58" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" s="7" customFormat="1">
       <c r="A58" s="8">
         <v>38596</v>
       </c>
@@ -6691,7 +6707,7 @@
         <v>4996</v>
       </c>
     </row>
-    <row r="59" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" s="7" customFormat="1">
       <c r="A59" s="8">
         <v>38626</v>
       </c>
@@ -6764,7 +6780,7 @@
         <v>4711</v>
       </c>
     </row>
-    <row r="60" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" s="7" customFormat="1">
       <c r="A60" s="8">
         <v>38657</v>
       </c>
@@ -6837,7 +6853,7 @@
         <v>4128</v>
       </c>
     </row>
-    <row r="61" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" s="7" customFormat="1">
       <c r="A61" s="8">
         <v>38687</v>
       </c>
@@ -6910,7 +6926,7 @@
         <v>4852</v>
       </c>
     </row>
-    <row r="62" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" s="7" customFormat="1">
       <c r="A62" s="8">
         <v>38718</v>
       </c>
@@ -6983,7 +6999,7 @@
         <v>4215</v>
       </c>
     </row>
-    <row r="63" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" s="7" customFormat="1">
       <c r="A63" s="8">
         <v>38749</v>
       </c>
@@ -7056,7 +7072,7 @@
         <v>5231</v>
       </c>
     </row>
-    <row r="64" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" s="7" customFormat="1">
       <c r="A64" s="8">
         <v>38777</v>
       </c>
@@ -7129,7 +7145,7 @@
         <v>4022</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" s="7" customFormat="1">
       <c r="A65" s="8">
         <v>38808</v>
       </c>
@@ -7202,7 +7218,7 @@
         <v>5991</v>
       </c>
     </row>
-    <row r="66" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" s="7" customFormat="1">
       <c r="A66" s="8">
         <v>38838</v>
       </c>
@@ -7275,7 +7291,7 @@
         <v>5478</v>
       </c>
     </row>
-    <row r="67" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" s="7" customFormat="1">
       <c r="A67" s="8">
         <v>38869</v>
       </c>
@@ -7348,7 +7364,7 @@
         <v>5055</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" s="7" customFormat="1">
       <c r="A68" s="8">
         <v>38899</v>
       </c>
@@ -7421,7 +7437,7 @@
         <v>6018</v>
       </c>
     </row>
-    <row r="69" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" s="7" customFormat="1">
       <c r="A69" s="8">
         <v>38930</v>
       </c>
@@ -7494,7 +7510,7 @@
         <v>5974</v>
       </c>
     </row>
-    <row r="70" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" s="7" customFormat="1">
       <c r="A70" s="8">
         <v>38961</v>
       </c>
@@ -7567,7 +7583,7 @@
         <v>5540</v>
       </c>
     </row>
-    <row r="71" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" s="7" customFormat="1">
       <c r="A71" s="8">
         <v>38991</v>
       </c>
@@ -7640,7 +7656,7 @@
         <v>5260</v>
       </c>
     </row>
-    <row r="72" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" s="7" customFormat="1">
       <c r="A72" s="8">
         <v>39022</v>
       </c>
@@ -7713,7 +7729,7 @@
         <v>4522</v>
       </c>
     </row>
-    <row r="73" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" s="7" customFormat="1">
       <c r="A73" s="8">
         <v>39052</v>
       </c>
@@ -7786,7 +7802,7 @@
         <v>4292</v>
       </c>
     </row>
-    <row r="74" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" s="7" customFormat="1">
       <c r="A74" s="8">
         <v>39083</v>
       </c>
@@ -7859,7 +7875,7 @@
         <v>6012</v>
       </c>
     </row>
-    <row r="75" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" s="7" customFormat="1">
       <c r="A75" s="8">
         <v>39114</v>
       </c>
@@ -7932,7 +7948,7 @@
         <v>7173</v>
       </c>
     </row>
-    <row r="76" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" s="7" customFormat="1">
       <c r="A76" s="8">
         <v>39142</v>
       </c>
@@ -8005,7 +8021,7 @@
         <v>6570</v>
       </c>
     </row>
-    <row r="77" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" s="7" customFormat="1">
       <c r="A77" s="8">
         <v>39173</v>
       </c>
@@ -8078,7 +8094,7 @@
         <v>6295</v>
       </c>
     </row>
-    <row r="78" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" s="7" customFormat="1">
       <c r="A78" s="8">
         <v>39203</v>
       </c>
@@ -8151,7 +8167,7 @@
         <v>7232</v>
       </c>
     </row>
-    <row r="79" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" s="7" customFormat="1">
       <c r="A79" s="8">
         <v>39234</v>
       </c>
@@ -8224,7 +8240,7 @@
         <v>5406</v>
       </c>
     </row>
-    <row r="80" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" s="7" customFormat="1">
       <c r="A80" s="8">
         <v>39264</v>
       </c>
@@ -8297,7 +8313,7 @@
         <v>7091</v>
       </c>
     </row>
-    <row r="81" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" s="7" customFormat="1">
       <c r="A81" s="8">
         <v>39295</v>
       </c>
@@ -8370,7 +8386,7 @@
         <v>6673</v>
       </c>
     </row>
-    <row r="82" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" s="7" customFormat="1">
       <c r="A82" s="8">
         <v>39326</v>
       </c>
@@ -8443,7 +8459,7 @@
         <v>5287</v>
       </c>
     </row>
-    <row r="83" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" s="7" customFormat="1">
       <c r="A83" s="8">
         <v>39356</v>
       </c>
@@ -8516,7 +8532,7 @@
         <v>6301</v>
       </c>
     </row>
-    <row r="84" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" s="7" customFormat="1">
       <c r="A84" s="8">
         <v>39387</v>
       </c>
@@ -8589,7 +8605,7 @@
         <v>4736</v>
       </c>
     </row>
-    <row r="85" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" s="7" customFormat="1">
       <c r="A85" s="8">
         <v>39417</v>
       </c>
@@ -8662,7 +8678,7 @@
         <v>5572</v>
       </c>
     </row>
-    <row r="86" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" s="7" customFormat="1">
       <c r="A86" s="8">
         <v>39448</v>
       </c>
@@ -8735,7 +8751,7 @@
         <v>5157</v>
       </c>
     </row>
-    <row r="87" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" s="7" customFormat="1">
       <c r="A87" s="8">
         <v>39479</v>
       </c>
@@ -8808,7 +8824,7 @@
         <v>5207</v>
       </c>
     </row>
-    <row r="88" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" s="7" customFormat="1">
       <c r="A88" s="8">
         <v>39508</v>
       </c>
@@ -8881,7 +8897,7 @@
         <v>4332</v>
       </c>
     </row>
-    <row r="89" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" s="7" customFormat="1">
       <c r="A89" s="8">
         <v>39539</v>
       </c>
@@ -8954,7 +8970,7 @@
         <v>5632</v>
       </c>
     </row>
-    <row r="90" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" s="7" customFormat="1">
       <c r="A90" s="8">
         <v>39569</v>
       </c>
@@ -9027,7 +9043,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="91" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" s="7" customFormat="1">
       <c r="A91" s="8">
         <v>39600</v>
       </c>
@@ -9100,7 +9116,7 @@
         <v>3871</v>
       </c>
     </row>
-    <row r="92" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" s="7" customFormat="1">
       <c r="A92" s="8">
         <v>39630</v>
       </c>
@@ -9173,7 +9189,7 @@
         <v>4331</v>
       </c>
     </row>
-    <row r="93" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" s="7" customFormat="1">
       <c r="A93" s="8">
         <v>39661</v>
       </c>
@@ -9246,7 +9262,7 @@
         <v>5762</v>
       </c>
     </row>
-    <row r="94" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" s="7" customFormat="1">
       <c r="A94" s="8">
         <v>39692</v>
       </c>
@@ -9319,7 +9335,7 @@
         <v>5463</v>
       </c>
     </row>
-    <row r="95" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" s="7" customFormat="1">
       <c r="A95" s="8">
         <v>39722</v>
       </c>
@@ -9392,7 +9408,7 @@
         <v>6116</v>
       </c>
     </row>
-    <row r="96" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" s="7" customFormat="1">
       <c r="A96" s="8">
         <v>39753</v>
       </c>
@@ -9465,7 +9481,7 @@
         <v>5226</v>
       </c>
     </row>
-    <row r="97" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" s="7" customFormat="1">
       <c r="A97" s="8">
         <v>39783</v>
       </c>
@@ -9538,7 +9554,7 @@
         <v>4119</v>
       </c>
     </row>
-    <row r="98" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" s="7" customFormat="1">
       <c r="A98" s="8">
         <v>39814</v>
       </c>
@@ -9611,7 +9627,7 @@
         <v>4191</v>
       </c>
     </row>
-    <row r="99" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" s="7" customFormat="1">
       <c r="A99" s="8">
         <v>39845</v>
       </c>
@@ -9684,7 +9700,7 @@
         <v>4535</v>
       </c>
     </row>
-    <row r="100" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" s="7" customFormat="1">
       <c r="A100" s="8">
         <v>39873</v>
       </c>
@@ -9757,7 +9773,7 @@
         <v>4267</v>
       </c>
     </row>
-    <row r="101" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" s="7" customFormat="1">
       <c r="A101" s="8">
         <v>39904</v>
       </c>
@@ -9830,7 +9846,7 @@
         <v>3458</v>
       </c>
     </row>
-    <row r="102" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" s="7" customFormat="1">
       <c r="A102" s="8">
         <v>39934</v>
       </c>
@@ -9903,7 +9919,7 @@
         <v>2695</v>
       </c>
     </row>
-    <row r="103" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" s="7" customFormat="1">
       <c r="A103" s="8">
         <v>39965</v>
       </c>
@@ -9976,7 +9992,7 @@
         <v>3281</v>
       </c>
     </row>
-    <row r="104" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" s="7" customFormat="1">
       <c r="A104" s="8">
         <v>39995</v>
       </c>
@@ -10049,7 +10065,7 @@
         <v>4684</v>
       </c>
     </row>
-    <row r="105" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" s="7" customFormat="1">
       <c r="A105" s="8">
         <v>40026</v>
       </c>
@@ -10122,7 +10138,7 @@
         <v>5249</v>
       </c>
     </row>
-    <row r="106" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" s="7" customFormat="1">
       <c r="A106" s="8">
         <v>40057</v>
       </c>
@@ -10195,7 +10211,7 @@
         <v>7265</v>
       </c>
     </row>
-    <row r="107" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" s="7" customFormat="1">
       <c r="A107" s="8">
         <v>40087</v>
       </c>
@@ -10268,7 +10284,7 @@
         <v>5845</v>
       </c>
     </row>
-    <row r="108" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" s="7" customFormat="1">
       <c r="A108" s="8">
         <v>40118</v>
       </c>
@@ -10341,7 +10357,7 @@
         <v>5123</v>
       </c>
     </row>
-    <row r="109" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" s="7" customFormat="1">
       <c r="A109" s="8">
         <v>40148</v>
       </c>
@@ -10414,7 +10430,7 @@
         <v>5980</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23">
       <c r="A110" s="8">
         <v>40179</v>
       </c>
@@ -10487,7 +10503,7 @@
         <v>5605</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23">
       <c r="A111" s="8">
         <v>40210</v>
       </c>
@@ -10560,7 +10576,7 @@
         <v>6204</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23">
       <c r="A112" s="8">
         <v>40238</v>
       </c>
@@ -10633,7 +10649,7 @@
         <v>5982</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23">
       <c r="A113" s="8">
         <v>40269</v>
       </c>
@@ -10706,7 +10722,7 @@
         <v>5353</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23">
       <c r="A114" s="8">
         <v>40299</v>
       </c>
@@ -10779,7 +10795,7 @@
         <v>5393</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23">
       <c r="A115" s="8">
         <v>40330</v>
       </c>
@@ -10852,7 +10868,7 @@
         <v>6679</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23">
       <c r="A116" s="8">
         <v>40360</v>
       </c>
@@ -10925,7 +10941,7 @@
         <v>7233</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23">
       <c r="A117" s="8">
         <v>40391</v>
       </c>
@@ -10998,7 +11014,7 @@
         <v>6622</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23">
       <c r="A118" s="8">
         <v>40422</v>
       </c>
@@ -11071,7 +11087,7 @@
         <v>6544</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23">
       <c r="A119" s="8">
         <v>40452</v>
       </c>
@@ -11144,7 +11160,7 @@
         <v>6203</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23">
       <c r="A120" s="8">
         <v>40483</v>
       </c>
@@ -11217,7 +11233,7 @@
         <v>6088</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23">
       <c r="A121" s="8">
         <v>40513</v>
       </c>
@@ -11290,7 +11306,7 @@
         <v>7596</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23">
       <c r="A122" s="8">
         <v>40544</v>
       </c>
@@ -11363,7 +11379,7 @@
         <v>5469</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23">
       <c r="A123" s="8">
         <v>40575</v>
       </c>
@@ -11436,7 +11452,7 @@
         <v>7861</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23">
       <c r="A124" s="8">
         <v>40603</v>
       </c>
@@ -11509,7 +11525,7 @@
         <v>7970</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23">
       <c r="A125" s="8">
         <v>40634</v>
       </c>
@@ -11582,7 +11598,7 @@
         <v>7399</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23">
       <c r="A126" s="8">
         <v>40664</v>
       </c>
@@ -11655,7 +11671,7 @@
         <v>6049</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23">
       <c r="A127" s="8">
         <v>40695</v>
       </c>
@@ -11728,7 +11744,7 @@
         <v>6453</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23">
       <c r="A128" s="8">
         <v>40725</v>
       </c>
@@ -11801,7 +11817,7 @@
         <v>8156</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23">
       <c r="A129" s="8">
         <v>40756</v>
       </c>
@@ -11874,7 +11890,7 @@
         <v>8004</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23">
       <c r="A130" s="8">
         <v>40787</v>
       </c>
@@ -11947,7 +11963,7 @@
         <v>9275</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23">
       <c r="A131" s="8">
         <v>40817</v>
       </c>
@@ -12020,7 +12036,7 @@
         <v>8407</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23">
       <c r="A132" s="8">
         <v>40848</v>
       </c>
@@ -12093,7 +12109,7 @@
         <v>8757</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23">
       <c r="A133" s="8">
         <v>40878</v>
       </c>
@@ -12166,7 +12182,7 @@
         <v>8446</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23">
       <c r="A134" s="8">
         <v>40909</v>
       </c>
@@ -12239,7 +12255,7 @@
         <v>7433</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23">
       <c r="A135" s="8">
         <v>40940</v>
       </c>
@@ -12312,7 +12328,7 @@
         <v>9227</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23">
       <c r="A136" s="8">
         <v>40969</v>
       </c>
@@ -12385,7 +12401,7 @@
         <v>9165</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23">
       <c r="A137" s="8">
         <v>41000</v>
       </c>
@@ -12458,7 +12474,7 @@
         <v>7427</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23">
       <c r="A138" s="8">
         <v>41030</v>
       </c>
@@ -12531,7 +12547,7 @@
         <v>5518</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23">
       <c r="A139" s="8">
         <v>41061</v>
       </c>
@@ -12604,7 +12620,7 @@
         <v>10705</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23">
       <c r="A140" s="8">
         <v>41091</v>
       </c>
@@ -12677,7 +12693,7 @@
         <v>9317</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23">
       <c r="A141" s="8">
         <v>41122</v>
       </c>
@@ -12750,7 +12766,7 @@
         <v>11029</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23">
       <c r="A142" s="8">
         <v>41153</v>
       </c>
@@ -12823,7 +12839,7 @@
         <v>10006</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23">
       <c r="A143" s="8">
         <v>41183</v>
       </c>
@@ -12896,7 +12912,7 @@
         <v>10426</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23">
       <c r="A144" s="8">
         <v>41214</v>
       </c>
@@ -12969,7 +12985,7 @@
         <v>10300</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:23">
       <c r="A145" s="8">
         <v>41244</v>
       </c>
@@ -13042,7 +13058,7 @@
         <v>12093</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23">
       <c r="A146" s="8">
         <v>41275</v>
       </c>
@@ -13115,7 +13131,7 @@
         <v>9551</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23">
       <c r="A147" s="8">
         <v>41306</v>
       </c>
@@ -13188,7 +13204,7 @@
         <v>11031</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23">
       <c r="A148" s="8">
         <v>41334</v>
       </c>
@@ -13261,7 +13277,7 @@
         <v>8154</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23">
       <c r="A149" s="8">
         <v>41365</v>
       </c>
@@ -13334,7 +13350,7 @@
         <v>9789</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23">
       <c r="A150" s="8">
         <v>41395</v>
       </c>
@@ -13407,7 +13423,7 @@
         <v>7033</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23">
       <c r="A151" s="8">
         <v>41426</v>
       </c>
@@ -13480,7 +13496,7 @@
         <v>11561</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23">
       <c r="A152" s="8">
         <v>41456</v>
       </c>
@@ -13553,7 +13569,7 @@
         <v>12218</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23">
       <c r="A153" s="8">
         <v>41487</v>
       </c>
@@ -13626,7 +13642,7 @@
         <v>10492</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23">
       <c r="A154" s="8">
         <v>41518</v>
       </c>
@@ -13699,7 +13715,7 @@
         <v>12352</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23">
       <c r="A155" s="8">
         <v>41548</v>
       </c>
@@ -13772,7 +13788,7 @@
         <v>12047</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23">
       <c r="A156" s="8">
         <v>41579</v>
       </c>
@@ -13845,7 +13861,7 @@
         <v>9508</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23">
       <c r="A157" s="8">
         <v>41609</v>
       </c>
@@ -13918,7 +13934,7 @@
         <v>12966</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23">
       <c r="A158" s="8">
         <v>41640</v>
       </c>
@@ -13991,7 +14007,7 @@
         <v>9384</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23">
       <c r="A159" s="8">
         <v>41671</v>
       </c>
@@ -14064,7 +14080,7 @@
         <v>10308</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23">
       <c r="A160" s="8">
         <v>41699</v>
       </c>
@@ -14137,7 +14153,7 @@
         <v>11231</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23">
       <c r="A161" s="8">
         <v>41730</v>
       </c>
@@ -14210,7 +14226,7 @@
         <v>9902</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23">
       <c r="A162" s="8">
         <v>41760</v>
       </c>
@@ -14283,7 +14299,7 @@
         <v>7001</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23">
       <c r="A163" s="8">
         <v>41791</v>
       </c>
@@ -14356,7 +14372,7 @@
         <v>13042</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23">
       <c r="A164" s="8">
         <v>41821</v>
       </c>
@@ -14429,7 +14445,7 @@
         <v>11669</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23">
       <c r="A165" s="8">
         <v>41852</v>
       </c>
@@ -14502,7 +14518,7 @@
         <v>12852</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23">
       <c r="A166" s="8">
         <v>41883</v>
       </c>
@@ -14575,7 +14591,7 @@
         <v>12372</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23">
       <c r="A167" s="8">
         <v>41913</v>
       </c>
@@ -14648,7 +14664,7 @@
         <v>13139</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23">
       <c r="A168" s="8">
         <v>41944</v>
       </c>
@@ -14721,7 +14737,7 @@
         <v>11742</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23">
       <c r="A169" s="8">
         <v>41974</v>
       </c>
@@ -14794,7 +14810,7 @@
         <v>13233</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23">
       <c r="A170" s="8">
         <v>42005</v>
       </c>
@@ -14867,7 +14883,7 @@
         <v>10822</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23">
       <c r="A171" s="8">
         <v>42036</v>
       </c>
@@ -14940,7 +14956,7 @@
         <v>12007</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23">
       <c r="A172" s="8">
         <v>42064</v>
       </c>
@@ -15013,7 +15029,7 @@
         <v>8853</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23">
       <c r="A173" s="8">
         <v>42095</v>
       </c>
@@ -15086,7 +15102,7 @@
         <v>10220</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23">
       <c r="A174" s="8">
         <v>42125</v>
       </c>
@@ -15159,7 +15175,7 @@
         <v>11964</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23">
       <c r="A175" s="8">
         <v>42156</v>
       </c>
@@ -15232,7 +15248,7 @@
         <v>12023</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23">
       <c r="A176" s="8">
         <v>42186</v>
       </c>
@@ -15305,7 +15321,7 @@
         <v>14232</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23">
       <c r="A177" s="8">
         <v>42217</v>
       </c>
@@ -15378,7 +15394,7 @@
         <v>11918</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23">
       <c r="A178" s="8">
         <v>42248</v>
       </c>
@@ -15451,7 +15467,7 @@
         <v>11305</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23">
       <c r="A179" s="8">
         <v>42278</v>
       </c>
@@ -15524,7 +15540,7 @@
         <v>9063</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23">
       <c r="A180" s="8">
         <v>42309</v>
       </c>
@@ -15597,7 +15613,7 @@
         <v>9743</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23">
       <c r="A181" s="8">
         <v>42339</v>
       </c>
@@ -15670,7 +15686,7 @@
         <v>11902</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23">
       <c r="A182" s="8">
         <v>42370</v>
       </c>
@@ -15743,7 +15759,7 @@
         <v>8932</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23">
       <c r="A183" s="8">
         <v>42401</v>
       </c>
@@ -15816,7 +15832,7 @@
         <v>8446</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23">
       <c r="A184" s="8">
         <v>42430</v>
       </c>
@@ -15889,7 +15905,7 @@
         <v>6838</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23">
       <c r="A185" s="8">
         <v>42461</v>
       </c>
@@ -15962,7 +15978,7 @@
         <v>8076</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23">
       <c r="A186" s="8">
         <v>42491</v>
       </c>
@@ -16035,7 +16051,7 @@
         <v>7685</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23">
       <c r="A187" s="8">
         <v>42522</v>
       </c>
@@ -16108,7 +16124,7 @@
         <v>8420</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23">
       <c r="A188" s="8">
         <v>42552</v>
       </c>
@@ -16181,7 +16197,7 @@
         <v>8805</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23">
       <c r="A189" s="8">
         <v>42583</v>
       </c>
@@ -16254,7 +16270,7 @@
         <v>9476</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23">
       <c r="A190" s="8">
         <v>42614</v>
       </c>
@@ -16327,7 +16343,7 @@
         <v>7567</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23">
       <c r="A191" s="8">
         <v>42644</v>
       </c>
@@ -16400,7 +16416,7 @@
         <v>8246</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23">
       <c r="A192" s="8">
         <v>42675</v>
       </c>
@@ -16473,7 +16489,7 @@
         <v>9392</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23">
       <c r="A193" s="8">
         <v>42705</v>
       </c>
@@ -16546,7 +16562,7 @@
         <v>9411</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23">
       <c r="A194" s="8">
         <v>42736</v>
       </c>
@@ -16619,7 +16635,7 @@
         <v>8385</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23">
       <c r="A195" s="8">
         <v>42767</v>
       </c>
@@ -16692,7 +16708,7 @@
         <v>5507</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23">
       <c r="A196" s="8">
         <v>42795</v>
       </c>
@@ -16765,7 +16781,7 @@
         <v>7962</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23">
       <c r="A197" s="8">
         <v>42826</v>
       </c>
@@ -16838,7 +16854,7 @@
         <v>7503</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23">
       <c r="A198" s="8">
         <v>42856</v>
       </c>
@@ -16911,7 +16927,7 @@
         <v>8031</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23">
       <c r="A199" s="8">
         <v>42887</v>
       </c>
@@ -16984,7 +17000,7 @@
         <v>7770</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:23">
       <c r="A200" s="8">
         <v>42917</v>
       </c>
@@ -17057,7 +17073,7 @@
         <v>7935</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:23">
       <c r="A201" s="8">
         <v>42948</v>
       </c>
@@ -17130,7 +17146,7 @@
         <v>9114</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:23">
       <c r="A202" s="8">
         <v>42979</v>
       </c>
@@ -17203,7 +17219,7 @@
         <v>9170</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:23">
       <c r="A203" s="8">
         <v>43009</v>
       </c>
@@ -17276,7 +17292,7 @@
         <v>7988</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:23">
       <c r="A204" s="8">
         <v>43040</v>
       </c>
@@ -17349,7 +17365,7 @@
         <v>7433</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:23" ht="15" customHeight="1">
       <c r="A205" s="8">
         <v>43070</v>
       </c>
@@ -17422,7 +17438,7 @@
         <v>8501</v>
       </c>
     </row>
-    <row r="206" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:23" ht="15" customHeight="1">
       <c r="A206" s="8">
         <v>43101</v>
       </c>
@@ -17495,7 +17511,7 @@
         <v>7314</v>
       </c>
     </row>
-    <row r="207" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:23" ht="15" customHeight="1">
       <c r="A207" s="8">
         <v>43132</v>
       </c>
@@ -17568,7 +17584,7 @@
         <v>7645</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:23" ht="15" customHeight="1">
       <c r="A208" s="8">
         <v>43160</v>
       </c>
@@ -17641,7 +17657,7 @@
         <v>6716</v>
       </c>
     </row>
-    <row r="209" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:23" ht="15" customHeight="1">
       <c r="A209" s="8">
         <v>43191</v>
       </c>
@@ -17714,7 +17730,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="210" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:23" ht="15" customHeight="1">
       <c r="A210" s="8">
         <v>43221</v>
       </c>
@@ -17787,7 +17803,7 @@
         <v>8168</v>
       </c>
     </row>
-    <row r="211" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:23" ht="15" customHeight="1">
       <c r="A211" s="8">
         <v>43252</v>
       </c>
@@ -17860,7 +17876,7 @@
         <v>8202</v>
       </c>
     </row>
-    <row r="212" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:23" ht="15" customHeight="1">
       <c r="A212" s="8">
         <v>43282</v>
       </c>
@@ -17933,7 +17949,7 @@
         <v>11154</v>
       </c>
     </row>
-    <row r="213" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:23" ht="15" customHeight="1">
       <c r="A213" s="8">
         <v>43313</v>
       </c>
@@ -18006,7 +18022,7 @@
         <v>8729</v>
       </c>
     </row>
-    <row r="214" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:23" ht="15" customHeight="1">
       <c r="A214" s="8">
         <v>43344</v>
       </c>
@@ -18079,7 +18095,7 @@
         <v>8317</v>
       </c>
     </row>
-    <row r="215" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:23" ht="15" customHeight="1">
       <c r="A215" s="8">
         <v>43374</v>
       </c>
@@ -18152,7 +18168,7 @@
         <v>9142</v>
       </c>
     </row>
-    <row r="216" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:23" ht="15" customHeight="1">
       <c r="A216" s="8">
         <v>43405</v>
       </c>
@@ -18225,7 +18241,7 @@
         <v>8778</v>
       </c>
     </row>
-    <row r="217" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:23" ht="15" customHeight="1">
       <c r="A217" s="8">
         <v>43435</v>
       </c>
@@ -18298,7 +18314,7 @@
         <v>9203</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:23">
       <c r="A218" s="8">
         <v>43466</v>
       </c>
@@ -18371,7 +18387,7 @@
         <v>7951</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:23">
       <c r="A219" s="8">
         <v>43497</v>
       </c>
@@ -18444,7 +18460,7 @@
         <v>7918</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:23">
       <c r="A220" s="8">
         <v>43525</v>
       </c>
@@ -18517,7 +18533,7 @@
         <v>9688</v>
       </c>
     </row>
-    <row r="221" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:23" s="25" customFormat="1">
       <c r="A221" s="8">
         <v>43556</v>
       </c>
@@ -18590,7 +18606,7 @@
         <v>9463</v>
       </c>
     </row>
-    <row r="222" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:23" s="25" customFormat="1">
       <c r="A222" s="8">
         <v>43586</v>
       </c>
@@ -18663,7 +18679,7 @@
         <v>9864</v>
       </c>
     </row>
-    <row r="223" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:23" s="25" customFormat="1">
       <c r="A223" s="8">
         <v>43617</v>
       </c>
@@ -18736,7 +18752,7 @@
         <v>7680</v>
       </c>
     </row>
-    <row r="224" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:23" s="25" customFormat="1">
       <c r="A224" s="8">
         <v>43647</v>
       </c>
@@ -18809,7 +18825,7 @@
         <v>9832</v>
       </c>
     </row>
-    <row r="225" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:23" s="25" customFormat="1">
       <c r="A225" s="8">
         <v>43678</v>
       </c>
@@ -18882,7 +18898,7 @@
         <v>10016</v>
       </c>
     </row>
-    <row r="226" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:23" s="25" customFormat="1">
       <c r="A226" s="8">
         <v>43709</v>
       </c>
@@ -18955,7 +18971,7 @@
         <v>10261</v>
       </c>
     </row>
-    <row r="227" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:23" s="25" customFormat="1">
       <c r="A227" s="8">
         <v>43739</v>
       </c>
@@ -19028,7 +19044,7 @@
         <v>10708</v>
       </c>
     </row>
-    <row r="228" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:23" s="25" customFormat="1">
       <c r="A228" s="8">
         <v>43770</v>
       </c>
@@ -19101,7 +19117,7 @@
         <v>9657</v>
       </c>
     </row>
-    <row r="229" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:23" s="25" customFormat="1">
       <c r="A229" s="8">
         <v>43800</v>
       </c>
@@ -19174,7 +19190,7 @@
         <v>9244</v>
       </c>
     </row>
-    <row r="230" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:23" s="25" customFormat="1">
       <c r="A230" s="8">
         <v>43831</v>
       </c>
@@ -19247,7 +19263,7 @@
         <v>9464</v>
       </c>
     </row>
-    <row r="231" spans="1:23" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:23" s="25" customFormat="1">
       <c r="A231" s="8">
         <v>43862</v>
       </c>
@@ -19320,7 +19336,7 @@
         <v>11517</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:23">
       <c r="A232" s="8">
         <v>43891</v>
       </c>
@@ -19393,7 +19409,7 @@
         <v>6933</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:23">
       <c r="A233" s="8">
         <v>43922</v>
       </c>
@@ -19466,7 +19482,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:23">
       <c r="A234" s="8">
         <v>43952</v>
       </c>
@@ -19539,7 +19555,7 @@
         <v>7780</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:23">
       <c r="A235" s="8">
         <v>43983</v>
       </c>
@@ -19612,7 +19628,7 @@
         <v>9856</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:23">
       <c r="A236" s="8">
         <v>44013</v>
       </c>
@@ -19685,7 +19701,7 @@
         <v>10436</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:23">
       <c r="A237" s="8">
         <v>44044</v>
       </c>
@@ -19758,7 +19774,7 @@
         <v>9904</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:23">
       <c r="A238" s="8">
         <v>44075</v>
       </c>
@@ -19831,7 +19847,7 @@
         <v>10920</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:23">
       <c r="A239" s="8">
         <v>44105</v>
       </c>
@@ -19904,7 +19920,7 @@
         <v>9703</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:23">
       <c r="A240" s="8">
         <v>44136</v>
       </c>
@@ -19977,7 +19993,7 @@
         <v>9501</v>
       </c>
     </row>
-    <row r="241" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:23">
       <c r="A241" s="8">
         <v>44166</v>
       </c>
@@ -20050,7 +20066,7 @@
         <v>10311</v>
       </c>
     </row>
-    <row r="242" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:23">
       <c r="A242" s="8">
         <v>44197</v>
       </c>
@@ -20123,7 +20139,7 @@
         <v>9276</v>
       </c>
     </row>
-    <row r="243" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:23">
       <c r="A243" s="8">
         <v>44228</v>
       </c>
@@ -20196,7 +20212,7 @@
         <v>10955</v>
       </c>
     </row>
-    <row r="244" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:23">
       <c r="A244" s="8">
         <v>44256</v>
       </c>
@@ -20269,7 +20285,7 @@
         <v>10207</v>
       </c>
     </row>
-    <row r="245" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:23">
       <c r="A245" s="8">
         <v>44287</v>
       </c>
@@ -20342,7 +20358,7 @@
         <v>10791</v>
       </c>
     </row>
-    <row r="246" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:23">
       <c r="A246" s="40">
         <v>44317</v>
       </c>
@@ -20415,7 +20431,7 @@
         <v>8616</v>
       </c>
     </row>
-    <row r="247" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:23">
       <c r="A247" s="8">
         <v>44348</v>
       </c>
@@ -20488,7 +20504,7 @@
         <v>10803</v>
       </c>
     </row>
-    <row r="248" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:23">
       <c r="A248" s="8">
         <v>44378</v>
       </c>
@@ -20499,11 +20515,11 @@
         <v>3.9699999999999999E-2</v>
       </c>
       <c r="D248" s="26">
-        <v>0.09</v>
+        <v>0.13189999999999999</v>
       </c>
       <c r="E248" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>9.2599999999999988E-2</v>
+        <v>5.0699999999999995E-2</v>
       </c>
       <c r="F248" s="13">
         <v>3829.42</v>
@@ -20561,7 +20577,7 @@
         <v>12433</v>
       </c>
     </row>
-    <row r="249" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:23">
       <c r="A249" s="8">
         <v>44409</v>
       </c>
@@ -20572,11 +20588,11 @@
         <v>4.4400000000000002E-2</v>
       </c>
       <c r="D249" s="26">
-        <v>0.09</v>
+        <v>0.13189999999999999</v>
       </c>
       <c r="E249" s="19">
         <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
-        <v>7.7700000000000019E-2</v>
+        <v>3.5800000000000026E-2</v>
       </c>
       <c r="F249" s="13">
         <v>3821.54</v>
@@ -20594,7 +20610,7 @@
         <v>-0.29899999999999999</v>
       </c>
       <c r="K249" s="22">
-        <v>68.5</v>
+        <v>67.709999999999994</v>
       </c>
       <c r="L249" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
@@ -20634,16 +20650,29 @@
         <v>12690</v>
       </c>
     </row>
-    <row r="250" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:23">
       <c r="A250" s="8">
         <v>44440</v>
       </c>
-      <c r="B250" s="23"/>
-      <c r="C250" s="23"/>
-      <c r="D250" s="26"/>
-      <c r="E250" s="19"/>
-      <c r="F250" s="13"/>
-      <c r="G250" s="24"/>
+      <c r="B250" s="23">
+        <v>0.1211</v>
+      </c>
+      <c r="C250" s="23">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="D250" s="26">
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="E250" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>3.4300000000000025E-2</v>
+      </c>
+      <c r="F250" s="13">
+        <v>3822</v>
+      </c>
+      <c r="G250" s="24">
+        <v>1014980</v>
+      </c>
       <c r="H250" s="22">
         <v>-0.03</v>
       </c>
@@ -20654,7 +20683,7 @@
         <v>-0.28699999999999998</v>
       </c>
       <c r="K250" s="22">
-        <v>75.03</v>
+        <v>71.3</v>
       </c>
       <c r="L250" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
@@ -20694,20 +20723,41 @@
         <v>12278</v>
       </c>
     </row>
-    <row r="251" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:23">
       <c r="A251" s="8">
         <v>44470</v>
       </c>
-      <c r="B251" s="23"/>
-      <c r="C251" s="23"/>
-      <c r="D251" s="26"/>
-      <c r="E251" s="19"/>
-      <c r="F251" s="13"/>
-      <c r="G251" s="24"/>
-      <c r="H251" s="22"/>
-      <c r="I251" s="22"/>
-      <c r="J251" s="22"/>
-      <c r="K251" s="22"/>
+      <c r="B251" s="23">
+        <v>0.1179</v>
+      </c>
+      <c r="C251" s="23">
+        <v>4.58E-2</v>
+      </c>
+      <c r="D251" s="41">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E251" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>6.6700000000000009E-2</v>
+      </c>
+      <c r="F251" s="13">
+        <v>3773</v>
+      </c>
+      <c r="G251" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H251" s="22">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="I251" s="22">
+        <v>0.106</v>
+      </c>
+      <c r="J251" s="22">
+        <v>-0.192</v>
+      </c>
+      <c r="K251" s="22">
+        <v>81.22</v>
+      </c>
       <c r="L251" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>10</v>
@@ -20718,29 +20768,69 @@
       <c r="N251" s="14">
         <v>1</v>
       </c>
-      <c r="O251" s="15"/>
-      <c r="P251" s="15"/>
-      <c r="Q251" s="16"/>
-      <c r="R251" s="16"/>
-      <c r="S251" s="16"/>
-      <c r="T251" s="16"/>
-      <c r="U251" s="24"/>
-      <c r="W251" s="24"/>
-    </row>
-    <row r="252" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O251" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P251" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q251" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="R251" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S251" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T251" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="U251" s="24">
+        <v>60940</v>
+      </c>
+      <c r="V251" s="14">
+        <v>10038</v>
+      </c>
+      <c r="W251" s="24">
+        <v>10707</v>
+      </c>
+    </row>
+    <row r="252" spans="1:23">
       <c r="A252" s="8">
         <v>44501</v>
       </c>
-      <c r="B252" s="23"/>
-      <c r="C252" s="23"/>
-      <c r="D252" s="26"/>
-      <c r="E252" s="19"/>
-      <c r="F252" s="13"/>
-      <c r="G252" s="24"/>
-      <c r="H252" s="22"/>
-      <c r="I252" s="22"/>
-      <c r="J252" s="22"/>
-      <c r="K252" s="22"/>
+      <c r="B252" s="23">
+        <v>0.10829999999999999</v>
+      </c>
+      <c r="C252" s="23">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="D252" s="41">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E252" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>6.3899999999999985E-2</v>
+      </c>
+      <c r="F252" s="13">
+        <v>3903</v>
+      </c>
+      <c r="G252" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H252" s="22">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="I252" s="22">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="J252" s="22">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="K252" s="22">
+        <v>78.599999999999994</v>
+      </c>
       <c r="L252" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>11</v>
@@ -20751,29 +20841,69 @@
       <c r="N252" s="14">
         <v>2</v>
       </c>
-      <c r="O252" s="15"/>
-      <c r="P252" s="15"/>
-      <c r="Q252" s="16"/>
-      <c r="R252" s="16"/>
-      <c r="S252" s="16"/>
-      <c r="T252" s="16"/>
-      <c r="U252" s="24"/>
-      <c r="W252" s="24"/>
-    </row>
-    <row r="253" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O252" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="P252" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q252" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="R252" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S252" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T252" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="U252" s="24">
+        <v>60321</v>
+      </c>
+      <c r="V252" s="14">
+        <v>8066</v>
+      </c>
+      <c r="W252" s="24">
+        <v>9173</v>
+      </c>
+    </row>
+    <row r="253" spans="1:23">
       <c r="A253" s="8">
         <v>44531</v>
       </c>
-      <c r="B253" s="23"/>
-      <c r="C253" s="23"/>
-      <c r="D253" s="26"/>
-      <c r="E253" s="19"/>
-      <c r="F253" s="13"/>
-      <c r="G253" s="24"/>
-      <c r="H253" s="22"/>
-      <c r="I253" s="22"/>
-      <c r="J253" s="22"/>
-      <c r="K253" s="22"/>
+      <c r="B253" s="23">
+        <v>0.1101</v>
+      </c>
+      <c r="C253" s="23">
+        <v>5.62E-2</v>
+      </c>
+      <c r="D253" s="41">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E253" s="19">
+        <f>+Tabla33[[#This Row],[INFLATION]]+Tabla33[[#This Row],[DESEMPLEO]]-Tabla33[[#This Row],[PIB GROWTH]]</f>
+        <v>6.93E-2</v>
+      </c>
+      <c r="F253" s="13">
+        <v>3963</v>
+      </c>
+      <c r="G253" s="24">
+        <v>1014980</v>
+      </c>
+      <c r="H253" s="22">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="I253" s="22">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J253" s="22">
+        <v>-0.20599999999999999</v>
+      </c>
+      <c r="K253" s="22">
+        <v>71.69</v>
+      </c>
       <c r="L253" s="13">
         <f>+MONTH(Tabla33[[#This Row],[FECHA]])</f>
         <v>12</v>
@@ -20784,16 +20914,35 @@
       <c r="N253" s="14">
         <v>2</v>
       </c>
-      <c r="O253" s="15"/>
-      <c r="P253" s="15"/>
-      <c r="Q253" s="16"/>
-      <c r="R253" s="16"/>
-      <c r="S253" s="16"/>
-      <c r="T253" s="16"/>
-      <c r="U253" s="24"/>
-      <c r="W253" s="24"/>
-    </row>
-    <row r="254" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O253" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="P253" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q253" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="R253" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="S253" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T253" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="U253" s="24">
+        <v>77651</v>
+      </c>
+      <c r="V253" s="14">
+        <v>11643</v>
+      </c>
+      <c r="W253" s="24">
+        <v>9143</v>
+      </c>
+    </row>
+    <row r="254" spans="1:23">
       <c r="A254" s="8">
         <v>44562</v>
       </c>
@@ -20801,11 +20950,21 @@
       <c r="C254" s="27"/>
       <c r="D254" s="19"/>
       <c r="E254" s="19"/>
-      <c r="F254" s="28"/>
-      <c r="G254" s="29"/>
-      <c r="H254" s="22"/>
-      <c r="I254" s="22"/>
-      <c r="J254" s="22"/>
+      <c r="F254" s="28">
+        <v>4000</v>
+      </c>
+      <c r="G254" s="29">
+        <v>1117172</v>
+      </c>
+      <c r="H254" s="22">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="I254" s="22">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="J254" s="22">
+        <v>-0.3</v>
+      </c>
       <c r="K254" s="22"/>
       <c r="L254" s="28"/>
       <c r="M254" s="28"/>
@@ -20820,7 +20979,7 @@
       <c r="V254" s="29"/>
       <c r="W254" s="24"/>
     </row>
-    <row r="255" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:23">
       <c r="A255" s="8">
         <v>44593</v>
       </c>
@@ -20847,7 +21006,7 @@
       <c r="V255" s="29"/>
       <c r="W255" s="24"/>
     </row>
-    <row r="256" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:23">
       <c r="A256" s="8">
         <v>44621</v>
       </c>
@@ -20874,7 +21033,7 @@
       <c r="V256" s="29"/>
       <c r="W256" s="24"/>
     </row>
-    <row r="257" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:23">
       <c r="A257" s="8">
         <v>44652</v>
       </c>
@@ -20901,7 +21060,7 @@
       <c r="V257" s="29"/>
       <c r="W257" s="24"/>
     </row>
-    <row r="258" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:23">
       <c r="A258" s="8">
         <v>44682</v>
       </c>
@@ -20928,7 +21087,7 @@
       <c r="V258" s="29"/>
       <c r="W258" s="24"/>
     </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:23">
       <c r="A259" s="8">
         <v>44713</v>
       </c>
@@ -20955,7 +21114,7 @@
       <c r="V259" s="29"/>
       <c r="W259" s="24"/>
     </row>
-    <row r="260" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:23">
       <c r="A260" s="8">
         <v>44743</v>
       </c>
@@ -20982,7 +21141,7 @@
       <c r="V260" s="29"/>
       <c r="W260" s="24"/>
     </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:23">
       <c r="A261" s="8">
         <v>44774</v>
       </c>
@@ -21009,7 +21168,7 @@
       <c r="V261" s="29"/>
       <c r="W261" s="24"/>
     </row>
-    <row r="262" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:23">
       <c r="A262" s="8">
         <v>44805</v>
       </c>
@@ -21036,7 +21195,7 @@
       <c r="V262" s="29"/>
       <c r="W262" s="24"/>
     </row>
-    <row r="263" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:23">
       <c r="A263" s="8">
         <v>44835</v>
       </c>
@@ -21063,7 +21222,7 @@
       <c r="V263" s="29"/>
       <c r="W263" s="24"/>
     </row>
-    <row r="264" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:23">
       <c r="A264" s="8">
         <v>44866</v>
       </c>
@@ -21090,7 +21249,7 @@
       <c r="V264" s="29"/>
       <c r="W264" s="24"/>
     </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:23">
       <c r="A265" s="8">
         <v>44896</v>
       </c>
@@ -21117,7 +21276,7 @@
       <c r="V265" s="29"/>
       <c r="W265" s="24"/>
     </row>
-    <row r="266" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:23">
       <c r="A266" s="8">
         <v>44927</v>
       </c>
@@ -21144,7 +21303,7 @@
       <c r="V266" s="29"/>
       <c r="W266" s="24"/>
     </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:23">
       <c r="A267" s="8">
         <v>44958</v>
       </c>
@@ -21171,7 +21330,7 @@
       <c r="V267" s="29"/>
       <c r="W267" s="24"/>
     </row>
-    <row r="268" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:23">
       <c r="A268" s="8">
         <v>44986</v>
       </c>
@@ -21198,7 +21357,7 @@
       <c r="V268" s="29"/>
       <c r="W268" s="24"/>
     </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:23">
       <c r="A269" s="8">
         <v>45017</v>
       </c>
@@ -21225,7 +21384,7 @@
       <c r="V269" s="29"/>
       <c r="W269" s="24"/>
     </row>
-    <row r="270" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:23">
       <c r="A270" s="8">
         <v>45047</v>
       </c>
@@ -21252,7 +21411,7 @@
       <c r="V270" s="29"/>
       <c r="W270" s="24"/>
     </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:23">
       <c r="A271" s="8">
         <v>45078</v>
       </c>
@@ -21279,7 +21438,7 @@
       <c r="V271" s="29"/>
       <c r="W271" s="24"/>
     </row>
-    <row r="272" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:23">
       <c r="A272" s="8">
         <v>45108</v>
       </c>
@@ -21306,7 +21465,7 @@
       <c r="V272" s="29"/>
       <c r="W272" s="24"/>
     </row>
-    <row r="273" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:23">
       <c r="A273" s="8">
         <v>45139</v>
       </c>
@@ -21333,7 +21492,7 @@
       <c r="V273" s="29"/>
       <c r="W273" s="24"/>
     </row>
-    <row r="274" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:23">
       <c r="A274" s="8">
         <v>45170</v>
       </c>
@@ -21360,7 +21519,7 @@
       <c r="V274" s="29"/>
       <c r="W274" s="24"/>
     </row>
-    <row r="275" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:23">
       <c r="A275" s="8">
         <v>45200</v>
       </c>
@@ -21387,7 +21546,7 @@
       <c r="V275" s="29"/>
       <c r="W275" s="24"/>
     </row>
-    <row r="276" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:23">
       <c r="A276" s="8">
         <v>45231</v>
       </c>
@@ -21414,7 +21573,7 @@
       <c r="V276" s="29"/>
       <c r="W276" s="24"/>
     </row>
-    <row r="277" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:23">
       <c r="A277" s="8">
         <v>45261</v>
       </c>
@@ -21441,7 +21600,7 @@
       <c r="V277" s="29"/>
       <c r="W277" s="24"/>
     </row>
-    <row r="278" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:23">
       <c r="A278" s="8">
         <v>45292</v>
       </c>
@@ -21468,7 +21627,7 @@
       <c r="V278" s="29"/>
       <c r="W278" s="24"/>
     </row>
-    <row r="279" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:23">
       <c r="A279" s="8">
         <v>45323</v>
       </c>
@@ -21495,7 +21654,7 @@
       <c r="V279" s="29"/>
       <c r="W279" s="24"/>
     </row>
-    <row r="280" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:23">
       <c r="A280" s="8">
         <v>45352</v>
       </c>
@@ -21522,7 +21681,7 @@
       <c r="V280" s="29"/>
       <c r="W280" s="24"/>
     </row>
-    <row r="281" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:23">
       <c r="A281" s="8">
         <v>45383</v>
       </c>
@@ -21549,7 +21708,7 @@
       <c r="V281" s="29"/>
       <c r="W281" s="24"/>
     </row>
-    <row r="282" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:23">
       <c r="A282" s="8">
         <v>45413</v>
       </c>
@@ -21576,7 +21735,7 @@
       <c r="V282" s="29"/>
       <c r="W282" s="24"/>
     </row>
-    <row r="283" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:23">
       <c r="A283" s="8">
         <v>45444</v>
       </c>
@@ -21603,7 +21762,7 @@
       <c r="V283" s="29"/>
       <c r="W283" s="24"/>
     </row>
-    <row r="284" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:23">
       <c r="A284" s="8">
         <v>45474</v>
       </c>
@@ -21630,7 +21789,7 @@
       <c r="V284" s="29"/>
       <c r="W284" s="24"/>
     </row>
-    <row r="285" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:23">
       <c r="A285" s="8">
         <v>45505</v>
       </c>
@@ -21657,7 +21816,7 @@
       <c r="V285" s="29"/>
       <c r="W285" s="24"/>
     </row>
-    <row r="286" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:23">
       <c r="A286" s="8">
         <v>45536</v>
       </c>
@@ -21684,7 +21843,7 @@
       <c r="V286" s="29"/>
       <c r="W286" s="24"/>
     </row>
-    <row r="287" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:23">
       <c r="A287" s="8">
         <v>45566</v>
       </c>
@@ -21711,7 +21870,7 @@
       <c r="V287" s="29"/>
       <c r="W287" s="24"/>
     </row>
-    <row r="288" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:23">
       <c r="A288" s="8">
         <v>45597</v>
       </c>
@@ -21738,7 +21897,7 @@
       <c r="V288" s="29"/>
       <c r="W288" s="24"/>
     </row>
-    <row r="289" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:23">
       <c r="A289" s="8">
         <v>45627</v>
       </c>
@@ -21766,6 +21925,7 @@
       <c r="W289" s="24"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>